<commit_message>
- Added new figures exports and updated XLSX table
</commit_message>
<xml_diff>
--- a/SI_sample_data_processed.xlsx
+++ b/SI_sample_data_processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Manuscripts\Naticarius_gastropod_clumped_Holocene\Naticarius data analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7717DED-2CCB-4E76-8051-5DF777DF2863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9067324D-AF0E-4A2D-A024-8ED6FEF52EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BDF961E0-610E-4927-BCFC-17560C035C74}"/>
+    <workbookView xWindow="22932" yWindow="-4440" windowWidth="30936" windowHeight="16776" xr2:uid="{BDF961E0-610E-4927-BCFC-17560C035C74}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="173">
   <si>
     <t>season</t>
   </si>
@@ -545,6 +545,15 @@
   </si>
   <si>
     <t>d18Ow_95CL_season_horizon</t>
+  </si>
+  <si>
+    <t>Sea Surface d18Ow (all samples)</t>
+  </si>
+  <si>
+    <t>Bottom water d18Ow (all samples)</t>
+  </si>
+  <si>
+    <t>Seasonal range in d18Ow (all samples)</t>
   </si>
 </sst>
 </file>
@@ -1521,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9633AB-72FC-40EF-BB5E-962643F29304}">
-  <dimension ref="A1:AZ39"/>
+  <dimension ref="A1:AZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BB17" sqref="BB17"/>
+    <sheetView tabSelected="1" topLeftCell="AC6" workbookViewId="0">
+      <selection activeCell="AQ33" sqref="AQ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1802,7 @@
       <c r="W2" s="12">
         <v>13.926097150083701</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="12">
         <v>13.926097150083701</v>
       </c>
       <c r="Y2" s="2">
@@ -1951,7 +1960,7 @@
       <c r="W3" s="12">
         <v>11.973306033704199</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="12">
         <v>11.973306033704199</v>
       </c>
       <c r="Y3" s="2">
@@ -2109,7 +2118,7 @@
       <c r="W4" s="12">
         <v>12.975207901124</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="12">
         <v>12.975207901124</v>
       </c>
       <c r="Y4" s="2">
@@ -2425,7 +2434,7 @@
       <c r="W6" s="19">
         <v>13.973664797160801</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6" s="19">
         <v>13.973664797160801</v>
       </c>
       <c r="Y6" s="2">
@@ -2583,7 +2592,7 @@
       <c r="W7" s="19">
         <v>14.0942767609938</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="19">
         <v>14.0942767609938</v>
       </c>
       <c r="Y7" s="2">
@@ -2741,7 +2750,7 @@
       <c r="W8" s="19">
         <v>15.610380366206501</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8" s="19">
         <v>15.610380366206501</v>
       </c>
       <c r="Y8" s="2">
@@ -2899,7 +2908,7 @@
       <c r="W9" s="24">
         <v>11.938184525191099</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9" s="24">
         <v>11.938184525191099</v>
       </c>
       <c r="Y9" s="2">
@@ -3057,7 +3066,7 @@
       <c r="W10" s="12">
         <v>11.7127689952715</v>
       </c>
-      <c r="X10" s="2">
+      <c r="X10" s="12">
         <v>11.7127689952715</v>
       </c>
       <c r="Y10" s="2">
@@ -3215,7 +3224,7 @@
       <c r="W11" s="12">
         <v>11.792481582810501</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11" s="12">
         <v>11.792481582810501</v>
       </c>
       <c r="Y11" s="2">
@@ -3373,7 +3382,7 @@
       <c r="W12" s="12">
         <v>13.143316610279999</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="12">
         <v>13.143316610279999</v>
       </c>
       <c r="Y12" s="2">
@@ -3531,7 +3540,7 @@
       <c r="W13" s="12">
         <v>14.327850336967799</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13" s="12">
         <v>14.327850336967799</v>
       </c>
       <c r="Y13" s="2">
@@ -3689,7 +3698,7 @@
       <c r="W14" s="12">
         <v>11.8618958751289</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14" s="12">
         <v>11.8618958751289</v>
       </c>
       <c r="Y14" s="2">
@@ -4479,7 +4488,7 @@
       <c r="W19" s="19">
         <v>14.0687307907323</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X19" s="19">
         <v>14.0687307907323</v>
       </c>
       <c r="Y19" s="2">
@@ -4637,7 +4646,7 @@
       <c r="W20" s="24">
         <v>16.419672779749401</v>
       </c>
-      <c r="X20" s="2">
+      <c r="X20" s="24">
         <v>16.419672779749401</v>
       </c>
       <c r="Y20" s="2">
@@ -4795,7 +4804,7 @@
       <c r="W21" s="12">
         <v>14.450327581831599</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X21" s="12">
         <v>14.450327581831599</v>
       </c>
       <c r="Y21" s="2">
@@ -4953,7 +4962,7 @@
       <c r="W22" s="12">
         <v>13.4508920258536</v>
       </c>
-      <c r="X22" s="2">
+      <c r="X22" s="12">
         <v>13.4508920258536</v>
       </c>
       <c r="Y22" s="2">
@@ -5111,7 +5120,7 @@
       <c r="W23" s="12">
         <v>16.317378903711699</v>
       </c>
-      <c r="X23" s="2">
+      <c r="X23" s="12">
         <v>16.317378903711699</v>
       </c>
       <c r="Y23" s="2">
@@ -5269,7 +5278,7 @@
       <c r="W24" s="12">
         <v>14.120894656137301</v>
       </c>
-      <c r="X24" s="2">
+      <c r="X24" s="12">
         <v>14.120894656137301</v>
       </c>
       <c r="Y24" s="2">
@@ -6270,6 +6279,50 @@
       <c r="AV39" s="2">
         <f>SQRT(AV24^2+AV29^2)</f>
         <v>5.4622766510381968</v>
+      </c>
+    </row>
+    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y41" s="2">
+        <f>AVERAGEIFS(Y2:Y29,K2:K29,"=protoconch")</f>
+        <v>-1.5981900658911898</v>
+      </c>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2">
+        <f t="array" ref="AB41">SQRT(SUMSQ(IF(K2:K29="protoconch",AB2:AB29,"")))/SUMIFS(N2:N29,K2:K29,"=protoconch")</f>
+        <v>0.40541325758163055</v>
+      </c>
+    </row>
+    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y42" s="2">
+        <f>AVERAGEIFS(Y2:Y29,K2:K29,"&lt;&gt;protoconch")</f>
+        <v>-1.8470430135774392</v>
+      </c>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2">
+        <f t="array" ref="AB42">SQRT(SUMSQ(IF(K2:K29&lt;&gt;"protoconch",W2:W29,"")))/SUMIFS(N2:N29,K2:K29,"&lt;&gt;protoconch")</f>
+        <v>1.404965349358732</v>
+      </c>
+    </row>
+    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>172</v>
+      </c>
+      <c r="AP43" s="2">
+        <f>AP6-AP2</f>
+        <v>1.7732965041577122</v>
+      </c>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2">
+        <f>SQRT(((AQ6-AR6)/2)^2+((AQ2-AR2)/2)^2)</f>
+        <v>0.47796843663603356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updated XLSX table
</commit_message>
<xml_diff>
--- a/SI_sample_data_processed.xlsx
+++ b/SI_sample_data_processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Manuscripts\Naticarius_gastropod_clumped_Holocene\Naticarius data analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9067324D-AF0E-4A2D-A024-8ED6FEF52EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A023931-C64C-4792-B626-07592BAC444D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4440" windowWidth="30936" windowHeight="16776" xr2:uid="{BDF961E0-610E-4927-BCFC-17560C035C74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{BDF961E0-610E-4927-BCFC-17560C035C74}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="174">
   <si>
     <t>season</t>
   </si>
@@ -554,6 +554,9 @@
   </si>
   <si>
     <t>Seasonal range in d18Ow (all samples)</t>
+  </si>
+  <si>
+    <t>d18Ow +/- 95CL</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1105,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1155,6 +1158,8 @@
     <xf numFmtId="165" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1532,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9633AB-72FC-40EF-BB5E-962643F29304}">
   <dimension ref="A1:AZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC6" workbookViewId="0">
-      <selection activeCell="AQ33" sqref="AQ33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" activeCellId="3" sqref="Y1:Y1048576 AB1:AB1048576 C1:C1048576 B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,6 +1565,7 @@
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -6194,6 +6200,14 @@
         <f>SQRT(SUMSQ(W3,W11,W13,W21,W25))/SUM(N3,N11,N13,N21,N25)</f>
         <v>2.4378155078482306</v>
       </c>
+      <c r="Y33" s="3">
+        <f>AVERAGE(Y3,Y11,Y13,Y21,Y25)</f>
+        <v>-2.4072189739222201</v>
+      </c>
+      <c r="AB33" s="2">
+        <f>SQRT(SUMSQ(AB3,AB11,AB13,AB21,AB25))/SUM(S3,S11,S13,S21,S25)</f>
+        <v>6.9844045436998545</v>
+      </c>
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -6210,6 +6224,14 @@
       <c r="W34" s="2">
         <f>SQRT(SUMSQ(W6,W8,W15,W19))/SUM(N6,N8,N15,N19)</f>
         <v>3.1326164727686754</v>
+      </c>
+      <c r="Y34" s="3">
+        <f>AVERAGE(Y6,Y8,Y15,Y19)</f>
+        <v>-0.44494629137115727</v>
+      </c>
+      <c r="AB34" s="2">
+        <f>SQRT(SUMSQ(AB6,AB8,AB15,AB19))/SUM(S6,S8,S15,S19)</f>
+        <v>7.4946003545222659</v>
       </c>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.25">
@@ -6337,10 +6359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93E821D-F4FE-4F2B-BC93-8D14C76289BF}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="P2" sqref="P2:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6354,11 +6376,12 @@
     <col min="7" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>140</v>
       </c>
@@ -6389,17 +6412,26 @@
       <c r="J1" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="N1" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="O1" s="50" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P1" s="53" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>72</v>
       </c>
@@ -6430,17 +6462,27 @@
       <c r="J2" s="31">
         <v>13.143316610279999</v>
       </c>
-      <c r="K2" s="27">
+      <c r="K2" s="2">
+        <v>-1.94543842367914</v>
+      </c>
+      <c r="L2" s="2">
+        <v>-3.0284139655023101</v>
+      </c>
+      <c r="M2" s="27">
         <v>2</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P2" s="52" t="str">
+        <f>_xlfn.CONCAT(ROUND(K2,1), " ± ",ABS(ROUND(L2,1)))</f>
+        <v>-1.9 ± 3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>30</v>
       </c>
@@ -6471,17 +6513,27 @@
       <c r="J3" s="31">
         <v>11.7127689952715</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="2">
+        <v>-2.4507808911100999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>-2.6987946993712999</v>
+      </c>
+      <c r="M3" s="27">
         <v>3</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="N3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="O3" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P3" s="52" t="str">
+        <f t="shared" ref="P3:P21" si="0">_xlfn.CONCAT(ROUND(K3,1), " ± ",ABS(ROUND(L3,1)))</f>
+        <v>-2.5 ± 2.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>78</v>
       </c>
@@ -6512,17 +6564,27 @@
       <c r="J4" s="38">
         <v>12.5697929218917</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="2">
+        <v>-0.56374340802118394</v>
+      </c>
+      <c r="L4" s="2">
+        <v>-2.89626565020545</v>
+      </c>
+      <c r="M4" s="35">
         <v>3</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="N4" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="O4" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-0.6 ± 2.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>82</v>
       </c>
@@ -6553,17 +6615,27 @@
       <c r="J5" s="38">
         <v>12.572219688133201</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="2">
+        <v>-1.9310687901822701</v>
+      </c>
+      <c r="L5" s="2">
+        <v>-2.8968248129339198</v>
+      </c>
+      <c r="M5" s="35">
         <v>3</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="N5" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="O5" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.9 ± 2.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>39</v>
       </c>
@@ -6594,17 +6666,27 @@
       <c r="J6" s="31">
         <v>11.792481582810501</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="2">
+        <v>-0.33602062381616998</v>
+      </c>
+      <c r="L6" s="2">
+        <v>-2.7171616550254698</v>
+      </c>
+      <c r="M6" s="27">
         <v>3</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="N6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="O6" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-0.3 ± 2.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>89</v>
       </c>
@@ -6635,17 +6717,27 @@
       <c r="J7" s="38">
         <v>19.259190075096701</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="2">
+        <v>1.29834845934236</v>
+      </c>
+      <c r="L7" s="2">
+        <v>-4.43760139979186</v>
+      </c>
+      <c r="M7" s="35">
         <v>2</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="N7" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="35" t="s">
+      <c r="O7" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>1.3 ± 4.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>123</v>
       </c>
@@ -6676,17 +6768,27 @@
       <c r="J8" s="44">
         <v>16.419672779749401</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="2">
+        <v>-0.161722882071482</v>
+      </c>
+      <c r="L8" s="2">
+        <v>-3.7833347418777499</v>
+      </c>
+      <c r="M8" s="39">
         <v>2</v>
       </c>
-      <c r="L8" s="39" t="s">
+      <c r="N8" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="O8" s="39" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-0.2 ± 3.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>126</v>
       </c>
@@ -6717,17 +6819,27 @@
       <c r="J9" s="44">
         <v>14.0687307907323</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="2">
+        <v>-1.67991410591637</v>
+      </c>
+      <c r="L9" s="2">
+        <v>-3.2416430393392299</v>
+      </c>
+      <c r="M9" s="39">
         <v>2</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="N9" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="O9" s="39" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.7 ± 3.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>92</v>
       </c>
@@ -6758,17 +6870,27 @@
       <c r="J10" s="38">
         <v>14.465250919171201</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="2">
+        <v>-0.78465966874536197</v>
+      </c>
+      <c r="L10" s="2">
+        <v>-3.3330071242330002</v>
+      </c>
+      <c r="M10" s="35">
         <v>2</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="N10" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="O10" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-0.8 ± 3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>51</v>
       </c>
@@ -6799,17 +6921,27 @@
       <c r="J11" s="31">
         <v>11.8618958751289</v>
       </c>
-      <c r="K11" s="27">
+      <c r="K11" s="2">
+        <v>-2.5607808911101002</v>
+      </c>
+      <c r="L11" s="2">
+        <v>-2.73315573159653</v>
+      </c>
+      <c r="M11" s="27">
         <v>3</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="N11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="O11" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P11" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-2.6 ± 2.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>54</v>
       </c>
@@ -6840,17 +6972,27 @@
       <c r="J12" s="31">
         <v>14.327850336967799</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K12" s="2">
+        <v>-1.38507051001666</v>
+      </c>
+      <c r="L12" s="2">
+        <v>-3.3013480039096401</v>
+      </c>
+      <c r="M12" s="27">
         <v>2</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="N12" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="O12" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P12" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.4 ± 3.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>58</v>
       </c>
@@ -6881,17 +7023,27 @@
       <c r="J13" s="31">
         <v>13.4508920258536</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="2">
+        <v>-4.5778813957914704</v>
+      </c>
+      <c r="L13" s="2">
+        <v>-3.0992838769247899</v>
+      </c>
+      <c r="M13" s="27">
         <v>3</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="N13" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="27" t="s">
+      <c r="O13" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P13" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-4.6 ± 3.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>62</v>
       </c>
@@ -6922,17 +7074,27 @@
       <c r="J14" s="31">
         <v>16.317378903711699</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="2">
+        <v>-2.6446596687453598</v>
+      </c>
+      <c r="L14" s="2">
+        <v>-3.7597647243575301</v>
+      </c>
+      <c r="M14" s="27">
         <v>2</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="N14" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="27" t="s">
+      <c r="O14" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P14" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-2.6 ± 3.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>95</v>
       </c>
@@ -6963,17 +7125,27 @@
       <c r="J15" s="38">
         <v>12.619907253443399</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="2">
+        <v>-4.5545175152879001</v>
+      </c>
+      <c r="L15" s="2">
+        <v>-2.9078127312081499</v>
+      </c>
+      <c r="M15" s="35">
         <v>2</v>
       </c>
-      <c r="L15" s="35" t="s">
+      <c r="N15" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="O15" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P15" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-4.6 ± 2.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>65</v>
       </c>
@@ -7004,17 +7176,27 @@
       <c r="J16" s="31">
         <v>14.120894656137301</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K16" s="2">
+        <v>-2.9360033063533701</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-3.2536623631652799</v>
+      </c>
+      <c r="M16" s="27">
         <v>2</v>
       </c>
-      <c r="L16" s="27" t="s">
+      <c r="N16" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="M16" s="27" t="s">
+      <c r="O16" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P16" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-2.9 ± 3.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>98</v>
       </c>
@@ -7045,17 +7227,27 @@
       <c r="J17" s="38">
         <v>15.3099049634391</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="2">
+        <v>-0.58928751453466899</v>
+      </c>
+      <c r="L17" s="2">
+        <v>-3.5276278717601501</v>
+      </c>
+      <c r="M17" s="35">
         <v>2</v>
       </c>
-      <c r="L17" s="35" t="s">
+      <c r="N17" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="M17" s="35" t="s">
+      <c r="O17" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P17" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-0.6 ± 3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>101</v>
       </c>
@@ -7086,17 +7278,27 @@
       <c r="J18" s="38">
         <v>11.5121988200142</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="2">
+        <v>-2.1660206238161699</v>
+      </c>
+      <c r="L18" s="2">
+        <v>-2.6525803732751698</v>
+      </c>
+      <c r="M18" s="35">
         <v>3</v>
       </c>
-      <c r="L18" s="35" t="s">
+      <c r="N18" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="M18" s="35" t="s">
+      <c r="O18" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P18" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-2.2 ± 2.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>104</v>
       </c>
@@ -7127,17 +7329,27 @@
       <c r="J19" s="38">
         <v>11.691952856122599</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="2">
+        <v>-4.6160033063533703</v>
+      </c>
+      <c r="L19" s="2">
+        <v>-2.6939983539452999</v>
+      </c>
+      <c r="M19" s="35">
         <v>3</v>
       </c>
-      <c r="L19" s="35" t="s">
+      <c r="N19" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="35" t="s">
+      <c r="O19" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P19" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-4.6 ± 2.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>107</v>
       </c>
@@ -7168,17 +7380,27 @@
       <c r="J20" s="38">
         <v>13.6630006965457</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="2">
+        <v>-1.6527371410001299</v>
+      </c>
+      <c r="L20" s="2">
+        <v>-3.1481568425220501</v>
+      </c>
+      <c r="M20" s="35">
         <v>2</v>
       </c>
-      <c r="L20" s="35" t="s">
+      <c r="N20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="M20" s="35" t="s">
+      <c r="O20" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.7 ± 3.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>68</v>
       </c>
@@ -7209,15 +7431,41 @@
       <c r="J21" s="31">
         <v>14.450327581831599</v>
       </c>
-      <c r="K21" s="27">
+      <c r="K21" s="2">
+        <v>-4.0677490794902402</v>
+      </c>
+      <c r="L21" s="2">
+        <v>-3.3295685672422999</v>
+      </c>
+      <c r="M21" s="27">
         <v>2</v>
       </c>
-      <c r="L21" s="27" t="s">
+      <c r="N21" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M21" s="27" t="s">
+      <c r="O21" s="27" t="s">
         <v>28</v>
       </c>
+      <c r="P21" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-4.1 ± 3.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K25" s="3"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K26" s="3"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7227,15 +7475,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E6D8A1-7A81-4856-B06B-01E1C5C8F9B7}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>140</v>
       </c>
@@ -7264,16 +7512,25 @@
         <v>129</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O1" s="53" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>120</v>
       </c>
@@ -7301,17 +7558,27 @@
       <c r="I2" s="44">
         <v>11.938184525191099</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="2">
+        <v>-1.28649360321149</v>
+      </c>
+      <c r="K2" s="2">
+        <v>-2.75073376156478</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K2" s="39">
+      <c r="M2" s="39">
         <v>3</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="N2" s="39" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" s="52" t="str">
+        <f>_xlfn.CONCAT(ROUND(J2,1), " ± ",ABS(ROUND(K2,1)))</f>
+        <v>-1.3 ± 2.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>43</v>
       </c>
@@ -7339,17 +7606,27 @@
       <c r="I3" s="31">
         <v>12.975207901124</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="2">
+        <v>-1.8151225120646599</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-2.9896792398903198</v>
+      </c>
+      <c r="L3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="27">
+      <c r="M3" s="27">
         <v>3</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="N3" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3" s="52" t="str">
+        <f t="shared" ref="O3:O8" si="0">_xlfn.CONCAT(ROUND(J3,1), " ± ",ABS(ROUND(K3,1)))</f>
+        <v>-1.8 ± 3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>85</v>
       </c>
@@ -7377,17 +7654,27 @@
       <c r="I4" s="38">
         <v>16.8377254008176</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="2">
+        <v>-1.6250303811453699</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-3.8796602306031298</v>
+      </c>
+      <c r="L4" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="35">
+      <c r="M4" s="35">
         <v>2</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="N4" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.6 ± 3.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>48</v>
       </c>
@@ -7415,17 +7702,27 @@
       <c r="I5" s="49">
         <v>11.973306033704199</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="2">
+        <v>-1.69273714100013</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-2.7588262750470598</v>
+      </c>
+      <c r="L5" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="45">
+      <c r="M5" s="45">
         <v>3</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="N5" s="45" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.7 ± 2.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>111</v>
       </c>
@@ -7453,17 +7750,27 @@
       <c r="I6" s="44">
         <v>14.0942767609938</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="2">
+        <v>0.56599124385527599</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-3.2475292076022599</v>
+      </c>
+      <c r="L6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="39">
+      <c r="M6" s="39">
         <v>2</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="N6" s="39" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6 ± 3.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>114</v>
       </c>
@@ -7491,17 +7798,27 @@
       <c r="I7" s="44">
         <v>13.973664797160801</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="2">
+        <v>0.34534033125463798</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-3.21973843252553</v>
+      </c>
+      <c r="L7" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="39">
+      <c r="M7" s="39">
         <v>2</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="N7" s="39" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>0.3 ± 3.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>36</v>
       </c>
@@ -7529,17 +7846,27 @@
       <c r="I8" s="31">
         <v>13.926097150083701</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="2">
+        <v>-3.5334435714932</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-3.2087781451805699</v>
+      </c>
+      <c r="L8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="27">
+      <c r="M8" s="27">
         <v>2</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="N8" s="27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>-3.5 ± 3.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>117</v>
       </c>
@@ -7567,15 +7894,49 @@
       <c r="I9" s="44">
         <v>15.610380366206501</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="2">
+        <v>0.118532017198287</v>
+      </c>
+      <c r="K9" s="2">
+        <v>-3.5968618355314601</v>
+      </c>
+      <c r="L9" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="39">
+      <c r="M9" s="39">
         <v>2</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="N9" s="39" t="s">
         <v>110</v>
       </c>
+      <c r="O9" s="52" t="str">
+        <f>_xlfn.CONCAT(ROUND(J9,1), " ± ",ABS(ROUND(K9,1)))</f>
+        <v>0.1 ± 3.6</v>
+      </c>
+    </row>
+    <row r="18" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X18" s="52"/>
+    </row>
+    <row r="19" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X19" s="52"/>
+    </row>
+    <row r="20" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="52"/>
+    </row>
+    <row r="21" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X21" s="52"/>
+    </row>
+    <row r="22" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X22" s="52"/>
+    </row>
+    <row r="23" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X23" s="52"/>
+    </row>
+    <row r="24" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X24" s="52"/>
+    </row>
+    <row r="25" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X25" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>